<commit_message>
Correct code and updated sample data
Corrected code (replaced score 10 with generic variable n.n) and edited sample_pref.xlsx to include description about mentors' capacity and also show the matching results in green highlighting.
</commit_message>
<xml_diff>
--- a/sample_pref.xlsx
+++ b/sample_pref.xlsx
@@ -19,23 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>mentors</t>
   </si>
   <si>
-    <t>m4</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
-    <t>m1</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
     <t>mentees</t>
   </si>
   <si>
@@ -118,6 +106,24 @@
   </si>
   <si>
     <t>Example: 2, 6 in "e5-m1" cell represents that (i) m1 was e5's 2nd preferred mentor and that (ii) e5 was m1's 6th preferred mentee.</t>
+  </si>
+  <si>
+    <t>Mentors' capacities are represented in parentheses to mj. Example, m1 (3) represents that m1 can guide 3 mentees.</t>
+  </si>
+  <si>
+    <t>m4 (2)</t>
+  </si>
+  <si>
+    <t>m3 (1)</t>
+  </si>
+  <si>
+    <t>m1 (3)</t>
+  </si>
+  <si>
+    <t>m2 (1)</t>
+  </si>
+  <si>
+    <t>Green highlighted cells represent matched pairs.</t>
   </si>
 </sst>
 </file>
@@ -133,12 +139,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,17 +165,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,174 +480,214 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="5"/>
+      <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="5"/>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="9">
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="B11:B16"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A3:A9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>